<commit_message>
Regenerate results for all controllers
</commit_message>
<xml_diff>
--- a/results/resultsACC.xlsx
+++ b/results/resultsACC.xlsx
@@ -537,13 +537,13 @@
         <v>139</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0003801164627075195</v>
+        <v>0.0004098448753356933</v>
       </c>
       <c r="M2" t="n">
-        <v>0.08752274513244629</v>
+        <v>0.08551836013793945</v>
       </c>
       <c r="N2" t="n">
-        <v>9.274482727050781e-05</v>
+        <v>9.393692016601562e-05</v>
       </c>
     </row>
     <row r="3">
@@ -583,13 +583,13 @@
         <v>138</v>
       </c>
       <c r="L3" t="n">
-        <v>8.895421028137207e-05</v>
+        <v>8.559322357177735e-05</v>
       </c>
       <c r="M3" t="n">
-        <v>0.001195430755615234</v>
+        <v>0.003118276596069336</v>
       </c>
       <c r="N3" t="n">
-        <v>6.67572021484375e-05</v>
+        <v>5.197525024414062e-05</v>
       </c>
     </row>
     <row r="4">
@@ -629,13 +629,13 @@
         <v>127</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0002307085990905762</v>
+        <v>0.0003015847206115723</v>
       </c>
       <c r="M4" t="n">
-        <v>0.001306295394897461</v>
+        <v>0.003179311752319336</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0001103878021240234</v>
+        <v>0.0001177787780761719</v>
       </c>
     </row>
     <row r="5">
@@ -675,13 +675,13 @@
         <v>130</v>
       </c>
       <c r="L5" t="n">
-        <v>6.65602684020996e-05</v>
+        <v>7.24029541015625e-05</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0003340244293212891</v>
+        <v>0.0007503032684326172</v>
       </c>
       <c r="N5" t="n">
-        <v>4.792213439941406e-05</v>
+        <v>4.720687866210938e-05</v>
       </c>
     </row>
     <row r="6">
@@ -700,34 +700,34 @@
         <v>0.9983310152990265</v>
       </c>
       <c r="E6" t="n">
-        <v>0.97581317764804</v>
+        <v>0.9749791492910759</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9078014184397163</v>
+        <v>0.8958333333333334</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.8958333333333334</v>
       </c>
       <c r="H6" t="n">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="I6" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J6" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K6" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L6" t="n">
-        <v>0.01036910486221313</v>
+        <v>0.008928798437118531</v>
       </c>
       <c r="M6" t="n">
-        <v>0.04379367828369141</v>
+        <v>0.04216599464416504</v>
       </c>
       <c r="N6" t="n">
-        <v>0.007346153259277344</v>
+        <v>0.007203340530395508</v>
       </c>
     </row>
     <row r="7">
@@ -746,19 +746,19 @@
         <v>0.9983310152990265</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9766472060050042</v>
+        <v>0.97581317764804</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9084507042253521</v>
+        <v>0.9020979020979021</v>
       </c>
       <c r="G7" t="n">
         <v>0.8958333333333334</v>
       </c>
       <c r="H7" t="n">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="I7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J7" t="n">
         <v>15</v>
@@ -767,13 +767,13 @@
         <v>129</v>
       </c>
       <c r="L7" t="n">
-        <v>0.00776460862159729</v>
+        <v>0.01020641756057739</v>
       </c>
       <c r="M7" t="n">
-        <v>0.01401257514953613</v>
+        <v>0.1040611267089844</v>
       </c>
       <c r="N7" t="n">
-        <v>0.006487369537353516</v>
+        <v>0.006453037261962891</v>
       </c>
     </row>
     <row r="8">
@@ -813,13 +813,13 @@
         <v>129</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0004749677181243897</v>
+        <v>0.0007186317443847656</v>
       </c>
       <c r="M8" t="n">
-        <v>0.001566171646118164</v>
+        <v>0.009264707565307617</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0002293586730957031</v>
+        <v>0.0002360343933105469</v>
       </c>
     </row>
     <row r="9">
@@ -859,13 +859,13 @@
         <v>142</v>
       </c>
       <c r="L9" t="n">
-        <v>9.203720092773437e-05</v>
+        <v>0.0001060323715209961</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0002605915069580078</v>
+        <v>0.0005729198455810547</v>
       </c>
       <c r="N9" t="n">
-        <v>8.177757263183594e-05</v>
+        <v>8.296966552734375e-05</v>
       </c>
     </row>
     <row r="10">
@@ -905,13 +905,13 @@
         <v>84</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0003099143505096436</v>
+        <v>0.0005566618442535401</v>
       </c>
       <c r="M10" t="n">
-        <v>0.001926422119140625</v>
+        <v>0.003770351409912109</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0001528263092041016</v>
+        <v>0.0001456737518310547</v>
       </c>
     </row>
     <row r="11">
@@ -951,13 +951,13 @@
         <v>84</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0001063132286071777</v>
+        <v>0.0001553776264190674</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0005266666412353516</v>
+        <v>0.002080917358398438</v>
       </c>
       <c r="N11" t="n">
-        <v>7.653236389160156e-05</v>
+        <v>9.1552734375e-05</v>
       </c>
     </row>
     <row r="12">
@@ -997,13 +997,13 @@
         <v>73</v>
       </c>
       <c r="L12" t="n">
-        <v>0.001021363973617554</v>
+        <v>0.002225195169448853</v>
       </c>
       <c r="M12" t="n">
-        <v>0.004738807678222656</v>
+        <v>0.01387214660644531</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0005795955657958984</v>
+        <v>0.0006763935089111328</v>
       </c>
     </row>
     <row r="13">
@@ -1043,13 +1043,13 @@
         <v>129</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0004420299530029297</v>
+        <v>0.0004849436283111572</v>
       </c>
       <c r="M13" t="n">
-        <v>0.001163244247436523</v>
+        <v>0.001590251922607422</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0003767013549804688</v>
+        <v>0.0003821849822998047</v>
       </c>
     </row>
     <row r="14">
@@ -1089,13 +1089,13 @@
         <v>74</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0002114307880401611</v>
+        <v>0.0002855598926544189</v>
       </c>
       <c r="M14" t="n">
-        <v>0.004486560821533203</v>
+        <v>0.01058053970336914</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0001027584075927734</v>
+        <v>9.846687316894531e-05</v>
       </c>
     </row>
     <row r="15">
@@ -1135,13 +1135,13 @@
         <v>74</v>
       </c>
       <c r="L15" t="n">
-        <v>9.11710262298584e-05</v>
+        <v>0.0001470100879669189</v>
       </c>
       <c r="M15" t="n">
-        <v>0.001619100570678711</v>
+        <v>0.01251840591430664</v>
       </c>
       <c r="N15" t="n">
-        <v>7.224082946777344e-05</v>
+        <v>4.553794860839844e-05</v>
       </c>
     </row>
     <row r="16">
@@ -1181,13 +1181,13 @@
         <v>97</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0003938231468200684</v>
+        <v>0.000534229040145874</v>
       </c>
       <c r="M16" t="n">
-        <v>0.008455276489257812</v>
+        <v>0.007826328277587891</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0001351833343505859</v>
+        <v>0.0002019405364990234</v>
       </c>
     </row>
     <row r="17">
@@ -1227,13 +1227,13 @@
         <v>130</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0001533312797546387</v>
+        <v>0.0001687929630279541</v>
       </c>
       <c r="M17" t="n">
-        <v>0.002132415771484375</v>
+        <v>0.002122402191162109</v>
       </c>
       <c r="N17" t="n">
-        <v>0.0001049041748046875</v>
+        <v>0.0001037120819091797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>